<commit_message>
updated case study run 2 results
</commit_message>
<xml_diff>
--- a/case study 80(10%) run2.xlsx
+++ b/case study 80(10%) run2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Imperial College London\School Work\Year 4\Research project\GITTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="8_{5F261379-F35E-4EEE-9F6E-82B3E217254F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{90E8B293-1E1E-44BA-923C-8FC8C4601CA1}"/>
+  <xr:revisionPtr revIDLastSave="322" documentId="8_{5F261379-F35E-4EEE-9F6E-82B3E217254F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{441914B6-9B50-466D-85B8-7EA70BEA78EC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1669,10 +1669,10 @@
   <dimension ref="A1:AL257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H224" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Y117" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S239" sqref="S239"/>
+      <selection pane="bottomRight" activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28471,11 +28471,11 @@
         <v>0.32721211637787501</v>
       </c>
       <c r="AF224" s="2">
-        <f t="shared" si="23"/>
+        <f>(AB224+20.6)/19.32</f>
         <v>47.570056288683581</v>
       </c>
       <c r="AG224" s="2">
-        <f t="shared" si="24"/>
+        <f>(AD224+14.667)/18.4</f>
         <v>50.250807851211526</v>
       </c>
       <c r="AH224" s="2">
@@ -32542,12 +32542,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F19637432BAAAA4E8B613AD4CF549CCD" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1a882fa068e99a90637f35d72ee4199">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f35accf0-cd8f-4670-ac72-d44f2085032d" xmlns:ns4="95507c7c-a837-40bb-8a3d-470d6a1609d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9631af341c2920228165fa301a4a4d8" ns3:_="" ns4:_="">
     <xsd:import namespace="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
@@ -32756,6 +32750,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -32766,23 +32766,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52F98C6A-6E2B-4BF6-8703-E04FA02071EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="95507c7c-a837-40bb-8a3d-470d6a1609d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4B0319-238C-4454-93A9-8E43BAF33F53}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32801,6 +32784,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52F98C6A-6E2B-4BF6-8703-E04FA02071EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="95507c7c-a837-40bb-8a3d-470d6a1609d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09983B4B-13DF-4740-912A-5320730E36D4}">
   <ds:schemaRefs>

</xml_diff>